<commit_message>
updating the FreeCRM Project
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testData/FreeCRMtestData.xlsx
+++ b/src/main/java/com/crm/qa/testData/FreeCRMtestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitha\IdeaFrameworkProjects\src\main\java\com\crm\qa\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3434C060-2167-4124-B36D-E5C86DCC8E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07682556-C4D8-4A5A-9E42-5A383FA12D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5DD9A12A-5F1C-48A6-B4D3-836B5E867996}"/>
+    <workbookView xWindow="660" yWindow="780" windowWidth="7500" windowHeight="6000" xr2:uid="{5DD9A12A-5F1C-48A6-B4D3-836B5E867996}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>FirstName</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>Nitha</t>
+  </si>
+  <si>
+    <t>Sonith Ajmal</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
 </sst>
 </file>
@@ -439,16 +448,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7086C4D5-1531-4881-9C81-D59B9D841E24}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -504,6 +513,17 @@
       </c>
       <c r="C5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>